<commit_message>
this is my twentyfifth commit
</commit_message>
<xml_diff>
--- a/testData/TC_FastQuotesConfig.xlsx
+++ b/testData/TC_FastQuotesConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilr2\eclipse-workspace\UCPQ_Automation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D918E6-D43B-40D1-AEE2-57C321F25DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96886F44-07DA-4F88-B101-09FF1B23748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,7 +149,7 @@
     <t>Fast Quotes</t>
   </si>
   <si>
-    <t>FASTQUOTE-AFF A20-001</t>
+    <t>FASTQUOTE-AFF-A20-001</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
this is my twentysixth commit
</commit_message>
<xml_diff>
--- a/testData/TC_FastQuotesConfig.xlsx
+++ b/testData/TC_FastQuotesConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilr2\eclipse-workspace\UCPQ_Automation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96886F44-07DA-4F88-B101-09FF1B23748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95A7901-AEDD-4F7B-B662-7CD198EA987A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>FASTQUOTE-AFF-A20-001</t>
+  </si>
+  <si>
+    <t>Expected Label</t>
   </si>
 </sst>
 </file>
@@ -188,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +210,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -231,25 +246,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -259,18 +261,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -552,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -576,127 +577,133 @@
     <col min="18" max="18" width="22.15234375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.3828125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="32.53515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="6" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="U3" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -743,12 +750,17 @@
       <c r="T4" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="U4" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{147F5B5B-A653-4F7A-9371-88FE8BC0D8D7}"/>

</xml_diff>